<commit_message>
Refactor, re-do file selection and point loading
Refactoring code for refinement of devX and UX
</commit_message>
<xml_diff>
--- a/codes.xlsx
+++ b/codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmonighan\Documents\Professional\Projects\Code\Python\Survey_Pt_Code_Checker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmonighan\Documents\Professional\Projects\Code\Python\Survey_Pt_Code_Checker - 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A68DDD-6CD8-4AC9-AC4C-67DD5270C635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80CCEA3-D502-4929-BB1A-77D917DC9880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="297">
   <si>
     <t>BS</t>
   </si>
@@ -924,6 +924,9 @@
   </si>
   <si>
     <t>BRKLINE</t>
+  </si>
+  <si>
+    <t>AS PH</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1314,7 @@
   <dimension ref="A5:B565"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,7 +1353,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>120</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Input files and recieve output file with problematic points
</commit_message>
<xml_diff>
--- a/codes.xlsx
+++ b/codes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="297">
   <si>
     <t xml:space="preserve">ABUT</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">AC</t>
   </si>
   <si>
-    <t xml:space="preserve">ACRB1</t>
+    <t xml:space="preserve">ACRB</t>
   </si>
   <si>
     <t xml:space="preserve">AD</t>
@@ -667,9 +667,6 @@
     <t xml:space="preserve">XS</t>
   </si>
   <si>
-    <t xml:space="preserve">ACRB</t>
-  </si>
-  <si>
     <t xml:space="preserve">AWNING</t>
   </si>
   <si>
@@ -911,6 +908,9 @@
   </si>
   <si>
     <t xml:space="preserve">METAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENT</t>
   </si>
 </sst>
 </file>
@@ -1133,11 +1133,11 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A520" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B545" activeCellId="0" sqref="B545"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74.57"/>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>215</v>
+        <v>3</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,7 +2233,7 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2258,7 +2258,7 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2283,7 +2283,7 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2298,7 +2298,7 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2323,12 +2323,12 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,7 +2353,7 @@
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,7 +2363,7 @@
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2383,7 +2383,7 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2393,7 +2393,7 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2408,7 +2408,7 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2438,7 +2438,7 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2478,12 +2478,12 @@
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,7 +2493,7 @@
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2543,7 +2543,7 @@
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2553,7 +2553,7 @@
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2568,7 +2568,7 @@
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,7 +2598,7 @@
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,12 +2638,12 @@
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2673,7 +2673,7 @@
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2718,12 +2718,12 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2743,7 +2743,7 @@
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,7 +2753,7 @@
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,7 +2788,7 @@
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2803,12 +2803,12 @@
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2856,7 +2856,7 @@
         <v>208</v>
       </c>
       <c r="B342" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2866,7 +2866,7 @@
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>215</v>
+        <v>3</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2896,12 +2896,12 @@
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2921,7 +2921,7 @@
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2946,7 +2946,7 @@
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2961,27 +2961,27 @@
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3021,7 +3021,7 @@
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3036,17 +3036,17 @@
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3066,12 +3066,12 @@
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3111,17 +3111,17 @@
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,12 +3131,12 @@
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3146,7 +3146,7 @@
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3161,7 +3161,7 @@
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,7 +3181,7 @@
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3201,22 +3201,22 @@
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3226,7 +3226,7 @@
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3266,7 +3266,7 @@
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3316,7 +3316,7 @@
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,7 +3351,7 @@
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3451,7 +3451,7 @@
     </row>
     <row r="461" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3471,17 +3471,17 @@
     </row>
     <row r="465" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3521,7 +3521,7 @@
     </row>
     <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3541,7 +3541,7 @@
     </row>
     <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3551,7 +3551,7 @@
     </row>
     <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3561,7 +3561,7 @@
     </row>
     <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3596,7 +3596,7 @@
     </row>
     <row r="490" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3611,12 +3611,12 @@
     </row>
     <row r="493" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3636,12 +3636,12 @@
     </row>
     <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3666,7 +3666,7 @@
     </row>
     <row r="504" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3726,7 +3726,7 @@
     </row>
     <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3736,7 +3736,7 @@
     </row>
     <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3776,7 +3776,7 @@
     </row>
     <row r="526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3786,7 +3786,7 @@
     </row>
     <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3796,7 +3796,7 @@
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3811,25 +3811,25 @@
     </row>
     <row r="533" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B534" s="0" t="s">
         <v>290</v>
-      </c>
-      <c r="B534" s="0" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3839,36 +3839,38 @@
     </row>
     <row r="538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A544" s="4" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A544" s="4"/>
     </row>
     <row r="545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="4"/>

</xml_diff>